<commit_message>
Docs : EquipmentsDB 생성
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/EquipmentsDB_Sheet.xlsx
+++ b/Assets/Excel/Items/EquipmentsDB_Sheet.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E74A9B-3150-4452-A162-EBDE0EB979DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D38340-2A61-4904-9D5B-F13351967D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Entities" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>_health</t>
-  </si>
-  <si>
-    <t>_meleeAtk</t>
   </si>
   <si>
     <t>_magicAtk</t>
@@ -98,13 +95,25 @@
   <si>
     <t>Accessories</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_physicalAtk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Icons/Equipments/Accessories_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Prefabs/Equipments/Accessories_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +125,13 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -140,8 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -424,20 +443,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="22.75" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="4" max="4" width="43.25" customWidth="1"/>
     <col min="5" max="5" width="13.25" customWidth="1"/>
     <col min="6" max="6" width="15.75" customWidth="1"/>
-    <col min="7" max="7" width="23.625" customWidth="1"/>
+    <col min="7" max="7" width="42.5" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="10.375" customWidth="1"/>
+    <col min="12" max="12" width="11.875" customWidth="1"/>
     <col min="13" max="13" width="10.75" customWidth="1"/>
     <col min="15" max="15" width="11.5" customWidth="1"/>
     <col min="16" max="16" width="14.125" customWidth="1"/>
@@ -446,69 +466,75 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
       </c>
       <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>7</v>
-      </c>
-      <c r="S1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10201011</v>
+      </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -516,14 +542,17 @@
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="H2">
         <v>24</v>
       </c>
       <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
       </c>
       <c r="K2">
         <v>0</v>

</xml_diff>

<commit_message>
Feature : Item Grade에 RuneStone 등급 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/EquipmentsDB_Sheet.xlsx
+++ b/Assets/Excel/Items/EquipmentsDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFA514F-4A73-4933-818A-463BDF811E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813D6BAE-3149-47E9-9AEA-9813466A0A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>_health</t>
   </si>
@@ -191,10 +191,6 @@
   </si>
   <si>
     <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unique</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -536,7 +532,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -548,6 +544,7 @@
     <col min="6" max="6" width="13.25" customWidth="1"/>
     <col min="7" max="7" width="15.75" customWidth="1"/>
     <col min="8" max="8" width="42.5" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="14" max="14" width="11.875" customWidth="1"/>
     <col min="15" max="15" width="10.75" customWidth="1"/>
@@ -623,7 +620,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>10121011</v>
+        <v>10112011</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -653,10 +650,10 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" t="s">
         <v>47</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
       </c>
       <c r="M2">
         <v>0</v>

</xml_diff>